<commit_message>
Tweak to COVID study, fix incorrect Estmand xref
</commit_message>
<xml_diff>
--- a/source_data/NCT04320615/Roche_NCT04320615_COVID.xlsx
+++ b/source_data/NCT04320615/Roche_NCT04320615_COVID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/NCT04320615/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88952656-C159-0443-A45D-3E82130640ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5E97D8-D5CE-5A43-BD56-50CD46F38387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37280" yWindow="4440" windowWidth="56520" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="37340" yWindow="4560" windowWidth="56520" windowHeight="19480" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="364">
   <si>
     <t>Epoch</t>
   </si>
@@ -606,9 +606,6 @@
     <t>IND2</t>
   </si>
   <si>
-    <t>INT2</t>
-  </si>
-  <si>
     <t>objectiveXref</t>
   </si>
   <si>
@@ -1132,6 +1129,18 @@
   </si>
   <si>
     <t>None set</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>IND3</t>
+  </si>
+  <si>
+    <t>IND4</t>
+  </si>
+  <si>
+    <t>SPONSOR:RO-4877533=Tocilizumab</t>
   </si>
 </sst>
 </file>
@@ -1306,10 +1315,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1630,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1679,66 +1688,66 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>202</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>217</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="C9" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="E9" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="F9" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="G9" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="H9" s="22" t="s">
         <v>210</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>216</v>
-      </c>
       <c r="D10" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1748,21 +1757,21 @@
         <v>43908</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B11" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>216</v>
-      </c>
       <c r="D11" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -1772,21 +1781,21 @@
         <v>43935</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>216</v>
-      </c>
       <c r="D12" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -1796,7 +1805,7 @@
         <v>43993</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1808,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1904,62 +1913,62 @@
         <v>182</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>330</v>
-      </c>
       <c r="D1" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="27" t="s">
         <v>239</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D2" t="s">
         <v>241</v>
       </c>
-      <c r="B2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>242</v>
-      </c>
-      <c r="E2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" t="s">
         <v>244</v>
       </c>
-      <c r="B3" t="s">
-        <v>333</v>
-      </c>
-      <c r="C3" t="s">
-        <v>334</v>
-      </c>
-      <c r="D3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="G3" t="s">
         <v>246</v>
-      </c>
-      <c r="G3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1993,56 +2002,56 @@
         <v>182</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="30" t="s">
         <v>258</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>39</v>
@@ -2051,81 +2060,81 @@
         <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>263</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>48</v>
@@ -2134,18 +2143,18 @@
         <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>49</v>
@@ -2154,18 +2163,18 @@
         <v>49</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>50</v>
@@ -2174,18 +2183,18 @@
         <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>51</v>
@@ -2194,18 +2203,18 @@
         <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>52</v>
@@ -2214,21 +2223,21 @@
         <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>263</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>53</v>
@@ -2237,18 +2246,18 @@
         <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>54</v>
@@ -2257,18 +2266,18 @@
         <v>54</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>55</v>
@@ -2277,18 +2286,18 @@
         <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>56</v>
@@ -2297,13 +2306,13 @@
         <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2333,7 +2342,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>57</v>
@@ -2342,18 +2351,18 @@
         <v>57</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>58</v>
@@ -2362,18 +2371,18 @@
         <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>59</v>
@@ -2382,18 +2391,18 @@
         <v>59</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>6</v>
@@ -2402,18 +2411,18 @@
         <v>6</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>60</v>
@@ -2422,18 +2431,18 @@
         <v>60</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>61</v>
@@ -2442,18 +2451,18 @@
         <v>61</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>62</v>
@@ -2462,18 +2471,18 @@
         <v>62</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>63</v>
@@ -2482,18 +2491,18 @@
         <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>64</v>
@@ -2502,18 +2511,18 @@
         <v>64</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>65</v>
@@ -2522,18 +2531,18 @@
         <v>65</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>66</v>
@@ -2542,18 +2551,18 @@
         <v>66</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>67</v>
@@ -2562,18 +2571,18 @@
         <v>67</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>68</v>
@@ -2582,18 +2591,18 @@
         <v>68</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>69</v>
@@ -2602,18 +2611,18 @@
         <v>69</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>70</v>
@@ -2622,18 +2631,18 @@
         <v>70</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>71</v>
@@ -2642,18 +2651,18 @@
         <v>71</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>72</v>
@@ -2662,18 +2671,18 @@
         <v>72</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>75</v>
@@ -2682,18 +2691,18 @@
         <v>75</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>76</v>
@@ -2702,18 +2711,18 @@
         <v>76</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>77</v>
@@ -2722,33 +2731,33 @@
         <v>77</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2778,101 +2787,101 @@
         <v>182</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>308</v>
-      </c>
       <c r="D1" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="30" t="s">
         <v>258</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>318</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2893,34 +2902,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
         <v>223</v>
-      </c>
-      <c r="B1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2973,7 +2982,7 @@
         <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>104</v>
@@ -2990,7 +2999,7 @@
         <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E3" t="s">
         <v>105</v>
@@ -3007,7 +3016,7 @@
         <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E4" t="s">
         <v>103</v>
@@ -3040,10 +3049,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>325</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>326</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
@@ -3052,10 +3061,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>327</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>328</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
@@ -3066,43 +3075,43 @@
       <c r="A3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="B3" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
     </row>
     <row r="4" spans="1:6" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="B4" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="B5" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
@@ -3113,7 +3122,7 @@
         <v>116</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
@@ -3124,7 +3133,7 @@
         <v>117</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
@@ -3132,10 +3141,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -3143,7 +3152,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -3159,7 +3168,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>118</v>
@@ -3182,19 +3191,19 @@
         <v>119</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>316</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3202,33 +3211,33 @@
         <v>120</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>316</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3254,19 +3263,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>346</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="30" t="s">
         <v>347</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>349</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3274,16 +3283,16 @@
         <v>119</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3291,16 +3300,16 @@
         <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3328,13 +3337,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3342,10 +3351,10 @@
         <v>118</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3353,10 +3362,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3364,10 +3373,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3375,10 +3384,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3386,10 +3395,10 @@
         <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3426,10 +3435,10 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>230</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>231</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>0</v>
@@ -3482,10 +3491,10 @@
     </row>
     <row r="2" spans="1:38" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>232</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>233</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>4</v>
@@ -3598,10 +3607,10 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>84</v>
@@ -4052,119 +4061,119 @@
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="G7" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AE7" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AF7" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AG7" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AI7" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="AJ7" s="1" t="s">
+      <c r="AK7" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AL7" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>45</v>
@@ -4222,7 +4231,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
@@ -4465,7 +4474,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
@@ -7370,10 +7379,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FA45D-9570-C643-AC7B-6310BD62121C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7413,7 +7422,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
         <v>129</v>
@@ -7427,7 +7436,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s">
         <v>129</v>
@@ -7441,7 +7450,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>362</v>
       </c>
       <c r="B5" t="s">
         <v>129</v>
@@ -7451,6 +7460,20 @@
       </c>
       <c r="D5" s="9" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>360</v>
+      </c>
+      <c r="C6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -7533,7 +7556,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>156</v>
@@ -7559,7 +7582,7 @@
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>145</v>
@@ -7582,7 +7605,7 @@
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>147</v>
@@ -7591,7 +7614,7 @@
         <v>166</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>162</v>
@@ -7607,7 +7630,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>148</v>
@@ -7624,7 +7647,7 @@
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>149</v>
@@ -7641,7 +7664,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>150</v>
@@ -7658,7 +7681,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>151</v>
@@ -7675,7 +7698,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>152</v>
@@ -7692,7 +7715,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>153</v>
@@ -7709,7 +7732,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>154</v>
@@ -7726,7 +7749,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>161</v>
@@ -7743,7 +7766,7 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>163</v>
@@ -7760,7 +7783,7 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>155</v>

</xml_diff>